<commit_message>
correct typo in models and preprocessinput file
</commit_message>
<xml_diff>
--- a/input/input_data.xlsx
+++ b/input/input_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jsdev\nodeproject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\trecktrafficsoftware\archiver\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="optional_inputs" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="calendar" sheetId="3" r:id="rId3"/>
     <sheet name="trip_times" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -831,17 +831,17 @@
     <t>10.45</t>
   </si>
   <si>
-    <t>22.08.2022</t>
-  </si>
-  <si>
-    <t>30.09.2022</t>
+    <t>01.02.2023</t>
+  </si>
+  <si>
+    <t>30.02.2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -853,7 +853,7 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1235,9 +1235,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1341,18 +1341,18 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.19921875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.8984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.59765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>-1.5814940598869101</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>-1.573822731061</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>11</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>-1.6176938676755499</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>12</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>-1.54098543947391</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>13</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>-1.573822731061</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>14</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>-1.63494913174836</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>15</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>16</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>-1.5796126738360099</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>19</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>20</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>22</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>-1.573822731061</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>23</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>-1.57264938488035</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>24</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>-1.573822731061</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>25</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>-1.573822731061</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>26</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>28</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>-1.5708145164060301</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>29</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>-1.5734860391568799</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>30</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>36</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>-1.60800188240558</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>37</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>-1.5763585447059101</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>38</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>40</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>41</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>42</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>-1.40097562958112</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>-1.6146873896624601</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>46</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>47</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>-1.5737639999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>50</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>-1.5955205064147799</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>51</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>-1.5731125321130499</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>54</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>-1.60724069279287</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>56</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>-1.5708145164060301</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>57</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>-1.5731125321130499</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>58</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>-1.5822603310585801</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>60</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>-1.5732204866085899</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>62</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>-1.5732204866085899</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>63</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>-1.5731125321130499</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>64</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>-1.5731125321130499</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>69</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>-1.5707168985689</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>70</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>-1.5737639999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>72</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>-1.5695825109522801</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>75</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>-1.58014906243315</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>76</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>-1.5504015839663401</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>77</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>-1.5707247728946601</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>78</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>-1.5707247728946601</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>80</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>-1.5707247728946601</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>81</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>-1.5707247728946601</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>82</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>-1.66142031455738</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>84</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>-1.57279574000983</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>85</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>-1.573822731061</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>86</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>-1.57279574000983</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>87</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>-1.5707247728946601</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>89</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>-1.5707247728946601</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>90</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>-1.56750405328137</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>91</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>-1.5493616345844501</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>92</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>-0.83248381264108795</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>93</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>-1.5772360000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>94</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>-1.5772360000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>95</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>-1.5772360000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>96</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>-1.57279574000983</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>97</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>-1.57279574000983</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>103</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>-1.61239539126888</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>105</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>108</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>-1.5606051317484899</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>109</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>-1.6071405470909299</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>110</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>-1.56999053964362</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>111</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>-1.5425367624575299</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>112</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>-1.5772360000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>113</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>-1.573822731061</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>115</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>116</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>-1.5737639999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>121</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>-1.54665828211898</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>122</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>-1.5781876605840499</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>123</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>-1.5772360000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>124</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>-1.5707247728946601</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>125</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>-1.5734484755904901</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>126</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>-1.56836300751538</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>130</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>-1.5728012979495301</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>131</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>-1.5728012979999999</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>132</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>-1.5732104436560801</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>133</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>-1.57294613724802</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>135</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>-1.5732104436560801</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>137</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>138</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>141</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>-1.56129997936438</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>142</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>-1.57286847962482</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>146</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>-1.57879891095253</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>147</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>148</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>-1.5728012979999999</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>152</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>153</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>155</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>157</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>-1.6285389740770699</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>158</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>-1.5721045589046601</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>160</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>-1.5947171605836099</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>161</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>-1.5625079029129301</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>166</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>-1.5575990532824</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>167</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>-1.6213631317484001</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>169</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>-1.573822731061</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>170</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>-1.60765119910503</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>172</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>175</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>-1.5737639999999999</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>177</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>-1.572872</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>178</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>-1.573822731061</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>179</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>-1.5709218047620499</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>180</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>-1.50908501640585</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>181</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>-1.5617091974596899</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>182</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>-1.57262617407732</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>183</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>-1.57419248211747</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>184</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>-1.572872</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>185</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>-1.572872</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>188</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>-1.6178277029127399</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>189</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>-1.5826215839667701</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>190</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>-1.5726002587348</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>193</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>-1.5790520029128201</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>194</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>196</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>-1.57419248211747</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>197</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>-1.59622138941962</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>198</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>-1.5758216251964701</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>200</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>-1.5757810029127901</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>201</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>-1.5728012979999999</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>202</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>-1.5757810029127901</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>203</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>-1.572872</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>204</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>-1.5728012979999999</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>206</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>-1.5757810029127901</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>207</v>
       </c>
@@ -4320,7 +4320,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>208</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>-1.5728012979999999</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>211</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>-1.5728012979999999</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>212</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>-1.5728012979999999</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>213</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>-1.5757810029127901</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>215</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>-1.5728012979999999</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>216</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>-1.5735769217589699</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>217</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>-1.5728012979999999</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>218</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>-1.5728012979999999</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>222</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>-1.5757702740772299</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>225</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>-1.5733838026385301</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>226</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>-1.9383303344579199</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>227</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>-1.572872</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>229</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>-1.5721045589046601</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>230</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>-1.5674825956101599</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>231</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>-1.572872</v>
       </c>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>232</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>-1.57292215794155</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>234</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>-1.5737639999999999</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>237</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>-1.57464309321273</v>
       </c>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>238</v>
       </c>
@@ -4757,7 +4757,7 @@
         <v>-1.5737639999999999</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>239</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>-1.57419248211747</v>
       </c>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>240</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>-1.6137186894665501</v>
       </c>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>241</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>-1.572872</v>
       </c>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>243</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>-1.572872</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>244</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>-1.58010614709074</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>245</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>-1.5967992278187</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>246</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>250</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>-1.5721045589046601</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>252</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>-1.5731729109528301</v>
       </c>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>253</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>-1.572872</v>
       </c>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>254</v>
       </c>
@@ -5010,7 +5010,7 @@
         <v>-1.5721045589046601</v>
       </c>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>260</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>-1.5709749454442401</v>
       </c>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>266</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>-1.60704967047685</v>
       </c>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>267</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>-1.5684488557310301</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>268</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>-1.5737639999999999</v>
       </c>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>269</v>
       </c>
@@ -5125,7 +5125,7 @@
         <v>-1.5737639999999999</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>272</v>
       </c>
@@ -5148,7 +5148,7 @@
         <v>-1.6238663317483999</v>
       </c>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>275</v>
       </c>
@@ -5171,7 +5171,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>277</v>
       </c>
@@ -5194,7 +5194,7 @@
         <v>-1.6335524974581099</v>
       </c>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>278</v>
       </c>
@@ -5217,7 +5217,7 @@
         <v>-1.56998896210167</v>
       </c>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>280</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>-1.57879891095253</v>
       </c>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>283</v>
       </c>
@@ -5263,7 +5263,7 @@
         <v>-1.5726420000000001</v>
       </c>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>285</v>
       </c>
@@ -5286,7 +5286,7 @@
         <v>-1.5716079999999999</v>
       </c>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>290</v>
       </c>
@@ -5309,7 +5309,7 @@
         <v>-1.5737639999999999</v>
       </c>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>291</v>
       </c>
@@ -5332,7 +5332,7 @@
         <v>-1.5758216251964701</v>
       </c>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>292</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>-1.62200758382768</v>
       </c>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>294</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>-1.5757702740772299</v>
       </c>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>295</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>-1.5757702740772299</v>
       </c>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>296</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>-1.5197396821370399</v>
       </c>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>297</v>
       </c>
@@ -5447,7 +5447,7 @@
         <v>-1.5757702740772299</v>
       </c>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>298</v>
       </c>
@@ -5470,7 +5470,7 @@
         <v>-1.5757702740772299</v>
       </c>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>299</v>
       </c>
@@ -5493,7 +5493,7 @@
         <v>-1.57879891095253</v>
       </c>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>301</v>
       </c>
@@ -5516,7 +5516,7 @@
         <v>-1.5757702740772299</v>
       </c>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>302</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>-1.5757702740772299</v>
       </c>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>303</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>-1.5757702740772299</v>
       </c>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>304</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>-1.5716079999999999</v>
       </c>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>305</v>
       </c>
@@ -5608,7 +5608,7 @@
         <v>-1.5716079999999999</v>
       </c>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>306</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>-1.5757702740772299</v>
       </c>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>307</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>-1.5716079999999999</v>
       </c>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>308</v>
       </c>
@@ -5677,7 +5677,7 @@
         <v>-1.57879891095253</v>
       </c>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>309</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>-1.5716079999999999</v>
       </c>
     </row>
-    <row r="190" spans="1:7">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>310</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>-1.5716079999999999</v>
       </c>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>311</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>-1.5716079999999999</v>
       </c>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>312</v>
       </c>
@@ -5769,7 +5769,7 @@
         <v>-1.57879891095253</v>
       </c>
     </row>
-    <row r="193" spans="1:7">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>314</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>-1.56375789482523</v>
       </c>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>316</v>
       </c>
@@ -5815,7 +5815,7 @@
         <v>-1.57879891095253</v>
       </c>
     </row>
-    <row r="195" spans="1:7">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>317</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>-1.57280608211679</v>
       </c>
     </row>
-    <row r="196" spans="1:7">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>318</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>-1.6231940605839901</v>
       </c>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>321</v>
       </c>
@@ -5884,7 +5884,7 @@
         <v>-1.5716079999999999</v>
       </c>
     </row>
-    <row r="198" spans="1:7">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>322</v>
       </c>
@@ -5907,7 +5907,7 @@
         <v>-1.6219889605839899</v>
       </c>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>323</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>-1.5716079999999999</v>
       </c>
     </row>
-    <row r="200" spans="1:7">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>324</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>-1.57290605208276</v>
       </c>
     </row>
-    <row r="201" spans="1:7">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>325</v>
       </c>
@@ -5976,7 +5976,7 @@
         <v>-1.6060059397888</v>
       </c>
     </row>
-    <row r="202" spans="1:7">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>326</v>
       </c>
@@ -5999,7 +5999,7 @@
         <v>-1.5721045589046601</v>
       </c>
     </row>
-    <row r="203" spans="1:7">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>327</v>
       </c>
@@ -6022,7 +6022,7 @@
         <v>-1.5707247728946601</v>
       </c>
     </row>
-    <row r="204" spans="1:7">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>329</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>-1.6147622262949901</v>
       </c>
     </row>
-    <row r="205" spans="1:7">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>330</v>
       </c>
@@ -6068,7 +6068,7 @@
         <v>-1.573822731061</v>
       </c>
     </row>
-    <row r="206" spans="1:7">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>331</v>
       </c>
@@ -6091,7 +6091,7 @@
         <v>-1.6146763956101799</v>
       </c>
     </row>
-    <row r="207" spans="1:7">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>334</v>
       </c>
@@ -6114,7 +6114,7 @@
         <v>-1.5757702740772299</v>
       </c>
     </row>
-    <row r="208" spans="1:7">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>335</v>
       </c>
@@ -6137,7 +6137,7 @@
         <v>-1.5742105740772501</v>
       </c>
     </row>
-    <row r="209" spans="1:7">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>337</v>
       </c>
@@ -6160,7 +6160,7 @@
         <v>-1.572872</v>
       </c>
     </row>
-    <row r="210" spans="1:7">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>338</v>
       </c>
@@ -6183,7 +6183,7 @@
         <v>-1.6220075834942</v>
       </c>
     </row>
-    <row r="211" spans="1:7">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>340</v>
       </c>
@@ -6206,7 +6206,7 @@
         <v>-1.5757702740772299</v>
       </c>
     </row>
-    <row r="212" spans="1:7">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>341</v>
       </c>
@@ -6229,7 +6229,7 @@
         <v>-1.5757702740772299</v>
       </c>
     </row>
-    <row r="213" spans="1:7">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>343</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>-1.5818458828064901</v>
       </c>
     </row>
-    <row r="214" spans="1:7">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>344</v>
       </c>
@@ -6275,7 +6275,7 @@
         <v>-1.5962857624332301</v>
       </c>
     </row>
-    <row r="215" spans="1:7">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>346</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>-1.57879891095253</v>
       </c>
     </row>
-    <row r="216" spans="1:7">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>347</v>
       </c>
@@ -6321,7 +6321,7 @@
         <v>-1.61501637592646</v>
       </c>
     </row>
-    <row r="217" spans="1:7">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>348</v>
       </c>
@@ -6344,7 +6344,7 @@
         <v>-1.6051521148549299</v>
       </c>
     </row>
-    <row r="218" spans="1:7">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>351</v>
       </c>
@@ -6367,7 +6367,7 @@
         <v>-1.57879891095253</v>
       </c>
     </row>
-    <row r="219" spans="1:7">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>352</v>
       </c>
@@ -6390,7 +6390,7 @@
         <v>-1.5716095452416201</v>
       </c>
     </row>
-    <row r="220" spans="1:7">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>354</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>-1.5758216251964701</v>
       </c>
     </row>
-    <row r="221" spans="1:7">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>355</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>-1.5758216251964701</v>
       </c>
     </row>
-    <row r="222" spans="1:7">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>356</v>
       </c>
@@ -6459,7 +6459,7 @@
         <v>-1.5758216251964701</v>
       </c>
     </row>
-    <row r="223" spans="1:7">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>357</v>
       </c>
@@ -6482,7 +6482,7 @@
         <v>-1.5758216251964701</v>
       </c>
     </row>
-    <row r="224" spans="1:7">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>360</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>-1.5721717814691001</v>
       </c>
     </row>
-    <row r="225" spans="1:7">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>361</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>-1.5758216251964701</v>
       </c>
     </row>
-    <row r="226" spans="1:7">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>363</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>-1.5758216251964701</v>
       </c>
     </row>
-    <row r="227" spans="1:7">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>365</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>-1.6210878839662799</v>
       </c>
     </row>
-    <row r="228" spans="1:7">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>368</v>
       </c>
@@ -6597,7 +6597,7 @@
         <v>-1.60705471640612</v>
       </c>
     </row>
-    <row r="229" spans="1:7">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>369</v>
       </c>
@@ -6620,7 +6620,7 @@
         <v>-1.5758216251964701</v>
       </c>
     </row>
-    <row r="230" spans="1:7">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>371</v>
       </c>
@@ -6643,7 +6643,7 @@
         <v>-1.5758216251964701</v>
       </c>
     </row>
-    <row r="231" spans="1:7">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>372</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>-1.5721045589046601</v>
       </c>
     </row>
-    <row r="232" spans="1:7">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>373</v>
       </c>
@@ -6689,7 +6689,7 @@
         <v>-1.57879891095253</v>
       </c>
     </row>
-    <row r="233" spans="1:7">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>374</v>
       </c>
@@ -6712,7 +6712,7 @@
         <v>-1.57879891095253</v>
       </c>
     </row>
-    <row r="234" spans="1:7">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>375</v>
       </c>
@@ -6748,14 +6748,14 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="12.09765625" customWidth="1"/>
-    <col min="10" max="10" width="13.69921875" customWidth="1"/>
-    <col min="11" max="11" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.125" customWidth="1"/>
+    <col min="10" max="10" width="13.75" customWidth="1"/>
+    <col min="11" max="11" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -6790,7 +6790,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -6841,13 +6841,13 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.09765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -6965,7 +6965,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -7024,7 +7024,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>4</v>
       </c>
@@ -7083,7 +7083,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>5</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>11</v>
       </c>
@@ -7201,7 +7201,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>12</v>
       </c>
@@ -7260,7 +7260,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>13</v>
       </c>
@@ -7319,7 +7319,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>14</v>
       </c>
@@ -7378,7 +7378,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>15</v>
       </c>
@@ -7437,7 +7437,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>16</v>
       </c>
@@ -7496,7 +7496,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>19</v>
       </c>
@@ -7555,7 +7555,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>20</v>
       </c>
@@ -7614,7 +7614,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>22</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>23</v>
       </c>
@@ -7732,7 +7732,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>24</v>
       </c>
@@ -7791,7 +7791,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>25</v>
       </c>
@@ -7850,7 +7850,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>26</v>
       </c>
@@ -7909,7 +7909,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>28</v>
       </c>
@@ -7968,7 +7968,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>29</v>
       </c>
@@ -8027,7 +8027,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>30</v>
       </c>
@@ -8086,7 +8086,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>36</v>
       </c>
@@ -8145,7 +8145,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>37</v>
       </c>
@@ -8204,7 +8204,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>38</v>
       </c>
@@ -8263,7 +8263,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>40</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>41</v>
       </c>
@@ -8381,7 +8381,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>42</v>
       </c>
@@ -8440,7 +8440,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>43</v>
       </c>
@@ -8499,7 +8499,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>44</v>
       </c>
@@ -8558,7 +8558,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>46</v>
       </c>
@@ -8617,7 +8617,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>47</v>
       </c>
@@ -8676,7 +8676,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>50</v>
       </c>
@@ -8735,7 +8735,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>51</v>
       </c>
@@ -8794,7 +8794,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>54</v>
       </c>
@@ -8853,7 +8853,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>56</v>
       </c>
@@ -8912,7 +8912,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>57</v>
       </c>
@@ -8971,7 +8971,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>58</v>
       </c>
@@ -9030,7 +9030,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:19">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>60</v>
       </c>
@@ -9089,7 +9089,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>62</v>
       </c>
@@ -9148,7 +9148,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>63</v>
       </c>
@@ -9207,7 +9207,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>64</v>
       </c>
@@ -9266,7 +9266,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>69</v>
       </c>
@@ -9325,7 +9325,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>70</v>
       </c>
@@ -9384,7 +9384,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:19">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>72</v>
       </c>
@@ -9443,7 +9443,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:19">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>75</v>
       </c>
@@ -9502,7 +9502,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:19">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>76</v>
       </c>
@@ -9561,7 +9561,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>77</v>
       </c>
@@ -9620,7 +9620,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:19">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>78</v>
       </c>
@@ -9679,7 +9679,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>80</v>
       </c>
@@ -9738,7 +9738,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:19">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>81</v>
       </c>
@@ -9797,7 +9797,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>82</v>
       </c>
@@ -9856,7 +9856,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>84</v>
       </c>
@@ -9915,7 +9915,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:19">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>85</v>
       </c>
@@ -9974,7 +9974,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:19">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>86</v>
       </c>
@@ -10033,7 +10033,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:19">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>87</v>
       </c>
@@ -10092,7 +10092,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:19">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>89</v>
       </c>
@@ -10151,7 +10151,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:19">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>90</v>
       </c>
@@ -10210,7 +10210,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:19">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>91</v>
       </c>
@@ -10269,7 +10269,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:19">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>92</v>
       </c>
@@ -10328,7 +10328,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:19">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>93</v>
       </c>
@@ -10387,7 +10387,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:19">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>94</v>
       </c>
@@ -10446,7 +10446,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:19">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>95</v>
       </c>
@@ -10505,7 +10505,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:19">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>96</v>
       </c>
@@ -10564,7 +10564,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:19">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>97</v>
       </c>
@@ -10623,7 +10623,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:19">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>103</v>
       </c>
@@ -10682,7 +10682,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:19">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>105</v>
       </c>
@@ -10741,7 +10741,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:19">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>108</v>
       </c>
@@ -10800,7 +10800,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:19">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>109</v>
       </c>
@@ -10859,7 +10859,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:19">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>110</v>
       </c>
@@ -10918,7 +10918,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:19">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>111</v>
       </c>
@@ -10977,7 +10977,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:19">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>112</v>
       </c>
@@ -11036,7 +11036,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:19">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>113</v>
       </c>
@@ -11095,7 +11095,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:19">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>115</v>
       </c>
@@ -11154,7 +11154,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:19">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>116</v>
       </c>
@@ -11213,7 +11213,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="75" spans="1:19">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>121</v>
       </c>
@@ -11272,7 +11272,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:19">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>122</v>
       </c>
@@ -11331,7 +11331,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:19">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>123</v>
       </c>
@@ -11390,7 +11390,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="78" spans="1:19">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>124</v>
       </c>
@@ -11449,7 +11449,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="1:19">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>125</v>
       </c>
@@ -11508,7 +11508,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:19">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>126</v>
       </c>
@@ -11567,7 +11567,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="81" spans="1:19">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>130</v>
       </c>
@@ -11626,7 +11626,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:19">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>131</v>
       </c>
@@ -11685,7 +11685,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="83" spans="1:19">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>132</v>
       </c>
@@ -11744,7 +11744,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:19">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>133</v>
       </c>
@@ -11803,7 +11803,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="1:19">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>135</v>
       </c>
@@ -11862,7 +11862,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="86" spans="1:19">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>137</v>
       </c>
@@ -11921,7 +11921,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="87" spans="1:19">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>138</v>
       </c>
@@ -11980,7 +11980,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="88" spans="1:19">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>141</v>
       </c>
@@ -12039,7 +12039,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:19">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>142</v>
       </c>
@@ -12098,7 +12098,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:19">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>146</v>
       </c>
@@ -12157,7 +12157,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="91" spans="1:19">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>147</v>
       </c>
@@ -12216,7 +12216,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="92" spans="1:19">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>148</v>
       </c>
@@ -12275,7 +12275,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:19">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>152</v>
       </c>
@@ -12334,7 +12334,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="94" spans="1:19">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>153</v>
       </c>
@@ -12393,7 +12393,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:19">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A95" s="4">
         <v>155</v>
       </c>
@@ -12452,7 +12452,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:19">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
         <v>157</v>
       </c>
@@ -12511,7 +12511,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="97" spans="1:19">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A97" s="4">
         <v>158</v>
       </c>
@@ -12570,7 +12570,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="98" spans="1:19">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
         <v>160</v>
       </c>
@@ -12629,7 +12629,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="99" spans="1:19">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>161</v>
       </c>
@@ -12688,7 +12688,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="1:19">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>166</v>
       </c>
@@ -12747,7 +12747,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="101" spans="1:19">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
         <v>167</v>
       </c>
@@ -12806,7 +12806,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="102" spans="1:19">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>169</v>
       </c>
@@ -12865,7 +12865,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="103" spans="1:19">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A103" s="4">
         <v>170</v>
       </c>
@@ -12924,7 +12924,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="104" spans="1:19">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
         <v>172</v>
       </c>
@@ -12983,7 +12983,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="105" spans="1:19">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
         <v>175</v>
       </c>
@@ -13042,7 +13042,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="106" spans="1:19">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>177</v>
       </c>
@@ -13101,7 +13101,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="107" spans="1:19">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A107" s="4">
         <v>178</v>
       </c>
@@ -13160,7 +13160,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="108" spans="1:19">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>179</v>
       </c>
@@ -13219,7 +13219,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="109" spans="1:19">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A109" s="4">
         <v>180</v>
       </c>
@@ -13278,7 +13278,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:19">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A110" s="4">
         <v>181</v>
       </c>
@@ -13337,7 +13337,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="111" spans="1:19">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>182</v>
       </c>
@@ -13396,7 +13396,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="112" spans="1:19">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>183</v>
       </c>
@@ -13455,7 +13455,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="113" spans="1:19">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>184</v>
       </c>
@@ -13514,7 +13514,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="114" spans="1:19">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
         <v>185</v>
       </c>
@@ -13573,7 +13573,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="115" spans="1:19">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
         <v>188</v>
       </c>
@@ -13632,7 +13632,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="116" spans="1:19">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
         <v>189</v>
       </c>
@@ -13691,7 +13691,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="117" spans="1:19">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>190</v>
       </c>
@@ -13750,7 +13750,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="118" spans="1:19">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
         <v>193</v>
       </c>
@@ -13809,7 +13809,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="119" spans="1:19">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
         <v>194</v>
       </c>
@@ -13868,7 +13868,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="120" spans="1:19">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
         <v>196</v>
       </c>
@@ -13927,7 +13927,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="121" spans="1:19">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
         <v>197</v>
       </c>
@@ -13986,7 +13986,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="122" spans="1:19">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A122" s="4">
         <v>198</v>
       </c>
@@ -14045,7 +14045,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="123" spans="1:19">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
         <v>200</v>
       </c>
@@ -14104,7 +14104,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="124" spans="1:19">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
         <v>201</v>
       </c>
@@ -14163,7 +14163,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="125" spans="1:19">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A125" s="4">
         <v>202</v>
       </c>
@@ -14222,7 +14222,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="126" spans="1:19">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A126" s="4">
         <v>203</v>
       </c>
@@ -14281,7 +14281,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="127" spans="1:19">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A127" s="4">
         <v>204</v>
       </c>
@@ -14340,7 +14340,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="128" spans="1:19">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A128" s="4">
         <v>206</v>
       </c>
@@ -14399,7 +14399,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="129" spans="1:19">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A129" s="4">
         <v>207</v>
       </c>
@@ -14458,7 +14458,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="130" spans="1:19">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A130" s="4">
         <v>208</v>
       </c>
@@ -14517,7 +14517,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="131" spans="1:19">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A131" s="4">
         <v>211</v>
       </c>
@@ -14576,7 +14576,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="132" spans="1:19">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A132" s="4">
         <v>212</v>
       </c>
@@ -14635,7 +14635,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="133" spans="1:19">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A133" s="4">
         <v>213</v>
       </c>
@@ -14694,7 +14694,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="134" spans="1:19">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A134" s="4">
         <v>215</v>
       </c>
@@ -14753,7 +14753,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="135" spans="1:19">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A135" s="4">
         <v>216</v>
       </c>
@@ -14812,7 +14812,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="136" spans="1:19">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A136" s="4">
         <v>217</v>
       </c>
@@ -14871,7 +14871,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="137" spans="1:19">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A137" s="4">
         <v>218</v>
       </c>
@@ -14930,7 +14930,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="138" spans="1:19">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A138" s="4">
         <v>222</v>
       </c>
@@ -14989,7 +14989,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="139" spans="1:19">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A139" s="4">
         <v>225</v>
       </c>
@@ -15048,7 +15048,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="140" spans="1:19">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A140" s="4">
         <v>226</v>
       </c>
@@ -15107,7 +15107,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="141" spans="1:19">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A141" s="4">
         <v>227</v>
       </c>
@@ -15166,7 +15166,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="142" spans="1:19">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A142" s="4">
         <v>229</v>
       </c>
@@ -15225,7 +15225,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="143" spans="1:19">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A143" s="4">
         <v>230</v>
       </c>
@@ -15284,7 +15284,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="144" spans="1:19">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A144" s="4">
         <v>231</v>
       </c>
@@ -15343,7 +15343,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="145" spans="1:19">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A145" s="4">
         <v>232</v>
       </c>
@@ -15402,7 +15402,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="146" spans="1:19">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A146" s="4">
         <v>234</v>
       </c>
@@ -15461,7 +15461,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="147" spans="1:19">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A147" s="4">
         <v>237</v>
       </c>
@@ -15520,7 +15520,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="148" spans="1:19">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A148" s="4">
         <v>238</v>
       </c>
@@ -15579,7 +15579,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="149" spans="1:19">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A149" s="4">
         <v>239</v>
       </c>
@@ -15638,7 +15638,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="150" spans="1:19">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A150" s="4">
         <v>240</v>
       </c>
@@ -15697,7 +15697,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="151" spans="1:19">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A151" s="4">
         <v>241</v>
       </c>
@@ -15756,7 +15756,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="152" spans="1:19">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A152" s="4">
         <v>243</v>
       </c>
@@ -15815,7 +15815,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="153" spans="1:19">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A153" s="4">
         <v>244</v>
       </c>
@@ -15874,7 +15874,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="154" spans="1:19">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A154" s="4">
         <v>245</v>
       </c>
@@ -15933,7 +15933,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="155" spans="1:19">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A155" s="4">
         <v>246</v>
       </c>
@@ -15992,7 +15992,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="156" spans="1:19">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A156" s="4">
         <v>250</v>
       </c>
@@ -16051,7 +16051,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="157" spans="1:19">
+    <row r="157" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A157" s="4">
         <v>252</v>
       </c>
@@ -16110,7 +16110,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="158" spans="1:19">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A158" s="4">
         <v>253</v>
       </c>
@@ -16169,7 +16169,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="159" spans="1:19">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A159" s="4">
         <v>254</v>
       </c>
@@ -16228,7 +16228,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="160" spans="1:19">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A160" s="4">
         <v>260</v>
       </c>
@@ -16287,7 +16287,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="161" spans="1:19">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A161" s="4">
         <v>266</v>
       </c>
@@ -16346,7 +16346,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="162" spans="1:19">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A162" s="4">
         <v>267</v>
       </c>
@@ -16405,7 +16405,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="163" spans="1:19">
+    <row r="163" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A163" s="4">
         <v>268</v>
       </c>
@@ -16464,7 +16464,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="164" spans="1:19">
+    <row r="164" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A164" s="4">
         <v>269</v>
       </c>
@@ -16523,7 +16523,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="165" spans="1:19">
+    <row r="165" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A165" s="4">
         <v>272</v>
       </c>
@@ -16582,7 +16582,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="166" spans="1:19">
+    <row r="166" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A166" s="4">
         <v>275</v>
       </c>
@@ -16641,7 +16641,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="167" spans="1:19">
+    <row r="167" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A167" s="4">
         <v>277</v>
       </c>
@@ -16700,7 +16700,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="168" spans="1:19">
+    <row r="168" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A168" s="4">
         <v>278</v>
       </c>
@@ -16759,7 +16759,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="169" spans="1:19">
+    <row r="169" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A169" s="4">
         <v>280</v>
       </c>
@@ -16818,7 +16818,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="170" spans="1:19">
+    <row r="170" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A170" s="4">
         <v>283</v>
       </c>
@@ -16877,7 +16877,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="171" spans="1:19">
+    <row r="171" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A171" s="4">
         <v>285</v>
       </c>
@@ -16936,7 +16936,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="172" spans="1:19">
+    <row r="172" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A172" s="4">
         <v>290</v>
       </c>
@@ -16995,7 +16995,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="173" spans="1:19">
+    <row r="173" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A173" s="4">
         <v>291</v>
       </c>
@@ -17054,7 +17054,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="174" spans="1:19">
+    <row r="174" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A174" s="4">
         <v>292</v>
       </c>
@@ -17113,7 +17113,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="175" spans="1:19">
+    <row r="175" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A175" s="4">
         <v>294</v>
       </c>
@@ -17172,7 +17172,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="176" spans="1:19">
+    <row r="176" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A176" s="4">
         <v>295</v>
       </c>
@@ -17231,7 +17231,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="177" spans="1:19">
+    <row r="177" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A177" s="4">
         <v>296</v>
       </c>
@@ -17290,7 +17290,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="178" spans="1:19">
+    <row r="178" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A178" s="4">
         <v>297</v>
       </c>
@@ -17349,7 +17349,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="179" spans="1:19">
+    <row r="179" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A179" s="4">
         <v>298</v>
       </c>
@@ -17408,7 +17408,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="180" spans="1:19">
+    <row r="180" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A180" s="4">
         <v>299</v>
       </c>
@@ -17467,7 +17467,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="181" spans="1:19">
+    <row r="181" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A181" s="4">
         <v>301</v>
       </c>
@@ -17526,7 +17526,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="182" spans="1:19">
+    <row r="182" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A182" s="4">
         <v>302</v>
       </c>
@@ -17585,7 +17585,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="183" spans="1:19">
+    <row r="183" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A183" s="4">
         <v>303</v>
       </c>
@@ -17644,7 +17644,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="184" spans="1:19">
+    <row r="184" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A184" s="4">
         <v>304</v>
       </c>
@@ -17703,7 +17703,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="185" spans="1:19">
+    <row r="185" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A185" s="4">
         <v>305</v>
       </c>
@@ -17762,7 +17762,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="186" spans="1:19">
+    <row r="186" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A186" s="4">
         <v>306</v>
       </c>
@@ -17821,7 +17821,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="187" spans="1:19">
+    <row r="187" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A187" s="4">
         <v>307</v>
       </c>
@@ -17880,7 +17880,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="188" spans="1:19">
+    <row r="188" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A188" s="4">
         <v>308</v>
       </c>
@@ -17939,7 +17939,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="189" spans="1:19">
+    <row r="189" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A189" s="4">
         <v>309</v>
       </c>
@@ -17998,7 +17998,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="190" spans="1:19">
+    <row r="190" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A190" s="4">
         <v>310</v>
       </c>
@@ -18057,7 +18057,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="191" spans="1:19">
+    <row r="191" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A191" s="4">
         <v>311</v>
       </c>
@@ -18116,7 +18116,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="192" spans="1:19">
+    <row r="192" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A192" s="4">
         <v>312</v>
       </c>
@@ -18175,7 +18175,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="193" spans="1:19">
+    <row r="193" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A193" s="4">
         <v>314</v>
       </c>
@@ -18234,7 +18234,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="194" spans="1:19">
+    <row r="194" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A194" s="4">
         <v>316</v>
       </c>
@@ -18293,7 +18293,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="195" spans="1:19">
+    <row r="195" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A195" s="4">
         <v>317</v>
       </c>
@@ -18352,7 +18352,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="196" spans="1:19">
+    <row r="196" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A196" s="4">
         <v>318</v>
       </c>
@@ -18411,7 +18411,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="197" spans="1:19">
+    <row r="197" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A197" s="4">
         <v>321</v>
       </c>
@@ -18470,7 +18470,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="198" spans="1:19">
+    <row r="198" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A198" s="4">
         <v>322</v>
       </c>
@@ -18529,7 +18529,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="199" spans="1:19">
+    <row r="199" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A199" s="4">
         <v>323</v>
       </c>
@@ -18588,7 +18588,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="200" spans="1:19">
+    <row r="200" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A200" s="4">
         <v>324</v>
       </c>
@@ -18647,7 +18647,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="201" spans="1:19">
+    <row r="201" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A201" s="4">
         <v>325</v>
       </c>
@@ -18706,7 +18706,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="202" spans="1:19">
+    <row r="202" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A202" s="4">
         <v>326</v>
       </c>
@@ -18765,7 +18765,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="203" spans="1:19">
+    <row r="203" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A203" s="4">
         <v>327</v>
       </c>
@@ -18824,7 +18824,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="204" spans="1:19">
+    <row r="204" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A204" s="4">
         <v>329</v>
       </c>
@@ -18883,7 +18883,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="205" spans="1:19">
+    <row r="205" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A205" s="4">
         <v>330</v>
       </c>
@@ -18942,7 +18942,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="206" spans="1:19">
+    <row r="206" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A206" s="4">
         <v>331</v>
       </c>
@@ -19001,7 +19001,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="207" spans="1:19">
+    <row r="207" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A207" s="4">
         <v>334</v>
       </c>
@@ -19060,7 +19060,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="208" spans="1:19">
+    <row r="208" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A208" s="4">
         <v>335</v>
       </c>
@@ -19119,7 +19119,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="209" spans="1:19">
+    <row r="209" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A209" s="4">
         <v>337</v>
       </c>
@@ -19178,7 +19178,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="210" spans="1:19">
+    <row r="210" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A210" s="4">
         <v>338</v>
       </c>
@@ -19237,7 +19237,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="211" spans="1:19">
+    <row r="211" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A211" s="4">
         <v>340</v>
       </c>
@@ -19296,7 +19296,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="212" spans="1:19">
+    <row r="212" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A212" s="4">
         <v>341</v>
       </c>
@@ -19355,7 +19355,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="213" spans="1:19">
+    <row r="213" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A213" s="4">
         <v>343</v>
       </c>
@@ -19414,7 +19414,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="214" spans="1:19">
+    <row r="214" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A214" s="4">
         <v>344</v>
       </c>
@@ -19473,7 +19473,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="215" spans="1:19">
+    <row r="215" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A215" s="4">
         <v>346</v>
       </c>
@@ -19532,7 +19532,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="216" spans="1:19">
+    <row r="216" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A216" s="4">
         <v>347</v>
       </c>
@@ -19591,7 +19591,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="217" spans="1:19">
+    <row r="217" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A217" s="4">
         <v>348</v>
       </c>
@@ -19650,7 +19650,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="218" spans="1:19">
+    <row r="218" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A218" s="4">
         <v>351</v>
       </c>
@@ -19709,7 +19709,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="219" spans="1:19">
+    <row r="219" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A219" s="4">
         <v>352</v>
       </c>
@@ -19768,7 +19768,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="220" spans="1:19">
+    <row r="220" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A220" s="4">
         <v>354</v>
       </c>
@@ -19827,7 +19827,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="221" spans="1:19">
+    <row r="221" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A221" s="4">
         <v>355</v>
       </c>
@@ -19886,7 +19886,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="222" spans="1:19">
+    <row r="222" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A222" s="4">
         <v>356</v>
       </c>
@@ -19945,7 +19945,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="223" spans="1:19">
+    <row r="223" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A223" s="4">
         <v>357</v>
       </c>
@@ -20004,7 +20004,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="224" spans="1:19">
+    <row r="224" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A224" s="4">
         <v>360</v>
       </c>
@@ -20063,7 +20063,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="225" spans="1:19">
+    <row r="225" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A225" s="4">
         <v>361</v>
       </c>
@@ -20122,7 +20122,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="226" spans="1:19">
+    <row r="226" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A226" s="4">
         <v>363</v>
       </c>
@@ -20181,7 +20181,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="227" spans="1:19">
+    <row r="227" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A227" s="4">
         <v>365</v>
       </c>
@@ -20240,7 +20240,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="228" spans="1:19">
+    <row r="228" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A228" s="4">
         <v>368</v>
       </c>
@@ -20299,7 +20299,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="229" spans="1:19">
+    <row r="229" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A229" s="4">
         <v>369</v>
       </c>
@@ -20358,7 +20358,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="230" spans="1:19">
+    <row r="230" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A230" s="4">
         <v>371</v>
       </c>
@@ -20417,7 +20417,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="231" spans="1:19">
+    <row r="231" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A231" s="4">
         <v>372</v>
       </c>
@@ -20476,7 +20476,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="232" spans="1:19">
+    <row r="232" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A232" s="4">
         <v>373</v>
       </c>
@@ -20535,7 +20535,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="233" spans="1:19">
+    <row r="233" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A233" s="4">
         <v>374</v>
       </c>
@@ -20594,7 +20594,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="234" spans="1:19">
+    <row r="234" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A234" s="4">
         <v>375</v>
       </c>

</xml_diff>